<commit_message>
Update User Acceptance Testing AI.xlsx
</commit_message>
<xml_diff>
--- a/Testing Documents/User Acceptance Testing AI.xlsx
+++ b/Testing Documents/User Acceptance Testing AI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harra\Documents\Term-3-AI\Testing Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E60B78B-E0F2-4317-8C2C-1FEF3B65DBCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1975317-22F5-40AF-8107-C0B8392826B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8478DEDF-7F04-4077-B68D-9AFD543336D7}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="68">
   <si>
     <t>User Acceptance Testing</t>
   </si>
@@ -293,6 +293,24 @@
   </si>
   <si>
     <t>Application displays a predicted value within the range</t>
+  </si>
+  <si>
+    <t>Application does not run</t>
+  </si>
+  <si>
+    <t>1.Open application
+2.enter input values
+3.start the prediction process</t>
+  </si>
+  <si>
+    <t>Input values in expected range
+[0,42,52812.09301,15609.38091,138961.2505]</t>
+  </si>
+  <si>
+    <t>Statement</t>
+  </si>
+  <si>
+    <t>Prediction shown on screen</t>
   </si>
 </sst>
 </file>
@@ -471,18 +489,11 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -493,9 +504,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -514,6 +522,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -833,10 +847,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2178B82F-BB68-4BFB-9B21-BA48D972587D}">
-  <dimension ref="A1:Q16"/>
+  <dimension ref="A1:Q15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -849,7 +863,8 @@
     <col min="6" max="6" width="11.7109375" customWidth="1"/>
     <col min="7" max="7" width="29.7109375" customWidth="1"/>
     <col min="8" max="8" width="21.5703125" customWidth="1"/>
-    <col min="9" max="11" width="18.28515625" customWidth="1"/>
+    <col min="9" max="9" width="28" customWidth="1"/>
+    <col min="10" max="11" width="18.28515625" customWidth="1"/>
     <col min="12" max="12" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="12.85546875" customWidth="1"/>
     <col min="14" max="14" width="10" customWidth="1"/>
@@ -860,566 +875,557 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="21" customHeight="1">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
+      <c r="O1" s="12"/>
+      <c r="P1" s="12"/>
+      <c r="Q1" s="12"/>
     </row>
     <row r="2" spans="1:17" ht="21" customHeight="1">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
-      <c r="P2" s="3"/>
-      <c r="Q2" s="3"/>
+      <c r="A2" s="13"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="13"/>
+      <c r="M2" s="13"/>
+      <c r="N2" s="13"/>
+      <c r="O2" s="13"/>
+      <c r="P2" s="13"/>
+      <c r="Q2" s="13"/>
     </row>
     <row r="3" spans="1:17" ht="30">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="D3" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="E3" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="15" t="s">
+      <c r="F3" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="15" t="s">
+      <c r="G3" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="H3" s="15" t="s">
+      <c r="H3" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="15" t="s">
+      <c r="I3" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="J3" s="15" t="s">
+      <c r="J3" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="K3" s="15" t="s">
+      <c r="K3" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="L3" s="15" t="s">
+      <c r="L3" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="M3" s="15" t="s">
+      <c r="M3" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="N3" s="15" t="s">
+      <c r="N3" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="O3" s="15" t="s">
+      <c r="O3" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="P3" s="15" t="s">
+      <c r="P3" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="Q3" s="15" t="s">
+      <c r="Q3" s="11" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:17" s="1" customFormat="1" ht="101.45" customHeight="1">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6" t="s">
+      <c r="G4" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="H4" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6" t="s">
+      <c r="I4" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="L4" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="M4" s="6" t="s">
+      <c r="M4" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="N4" s="7" t="s">
+      <c r="N4" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="O4" s="6" t="s">
+      <c r="O4" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="P4" s="8">
+      <c r="P4" s="5">
         <v>45173</v>
       </c>
-      <c r="Q4" s="6"/>
+      <c r="Q4" s="3"/>
     </row>
-    <row r="5" spans="1:17" s="4" customFormat="1" ht="69.75" customHeight="1">
-      <c r="A5" s="5" t="s">
+    <row r="5" spans="1:17" ht="69.75" customHeight="1">
+      <c r="A5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
-      <c r="M5" s="6"/>
-      <c r="N5" s="7" t="s">
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="O5" s="6" t="s">
+      <c r="O5" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="P5" s="8">
+      <c r="P5" s="5">
         <v>45173</v>
       </c>
-      <c r="Q5" s="6"/>
+      <c r="Q5" s="3"/>
     </row>
     <row r="6" spans="1:17" ht="89.25" customHeight="1">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="5"/>
-      <c r="L6" s="5"/>
-      <c r="M6" s="5"/>
-      <c r="N6" s="7" t="s">
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="N6" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="O6" s="6" t="s">
+      <c r="O6" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="P6" s="8">
+      <c r="P6" s="5">
         <v>45173</v>
       </c>
-      <c r="Q6" s="5"/>
+      <c r="Q6" s="2"/>
     </row>
     <row r="7" spans="1:17" ht="51">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="E7" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="5"/>
-      <c r="M7" s="5"/>
-      <c r="N7" s="7" t="s">
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="O7" s="6" t="s">
+      <c r="O7" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="P7" s="8">
+      <c r="P7" s="5">
         <v>45173</v>
       </c>
-      <c r="Q7" s="5"/>
+      <c r="Q7" s="2"/>
     </row>
     <row r="8" spans="1:17" ht="70.5" customHeight="1">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E8" s="11" t="s">
+      <c r="E8" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="F8" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="5"/>
-      <c r="L8" s="5"/>
-      <c r="M8" s="5"/>
-      <c r="N8" s="7" t="s">
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="O8" s="6" t="s">
+      <c r="O8" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="P8" s="8">
+      <c r="P8" s="5">
         <v>45173</v>
       </c>
-      <c r="Q8" s="5"/>
+      <c r="Q8" s="2"/>
     </row>
     <row r="9" spans="1:17" ht="81.75" customHeight="1">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E9" s="11" t="s">
+      <c r="E9" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="F9" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="5"/>
-      <c r="L9" s="5"/>
-      <c r="M9" s="5"/>
-      <c r="N9" s="7" t="s">
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="O9" s="6" t="s">
+      <c r="O9" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="P9" s="8">
+      <c r="P9" s="5">
         <v>45173</v>
       </c>
-      <c r="Q9" s="5"/>
+      <c r="Q9" s="2"/>
     </row>
     <row r="10" spans="1:17" ht="84" customHeight="1">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E10" s="11" t="s">
+      <c r="E10" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="F10" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="5"/>
-      <c r="L10" s="5"/>
-      <c r="M10" s="5"/>
-      <c r="N10" s="7" t="s">
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="O10" s="6" t="s">
+      <c r="O10" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="P10" s="8">
+      <c r="P10" s="5">
         <v>45173</v>
       </c>
-      <c r="Q10" s="5"/>
+      <c r="Q10" s="2"/>
     </row>
     <row r="11" spans="1:17" ht="88.5" customHeight="1">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="E11" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="F11" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="5"/>
-      <c r="K11" s="5"/>
-      <c r="L11" s="5"/>
-      <c r="M11" s="5"/>
-      <c r="N11" s="7" t="s">
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="O11" s="6" t="s">
+      <c r="O11" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="P11" s="8">
+      <c r="P11" s="5">
         <v>45173</v>
       </c>
-      <c r="Q11" s="5"/>
+      <c r="Q11" s="2"/>
     </row>
     <row r="12" spans="1:17" ht="54.75" customHeight="1">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="C12" s="13" t="s">
+      <c r="C12" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E12" s="10" t="s">
+      <c r="E12" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="F12" s="6" t="s">
+      <c r="F12" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="5"/>
-      <c r="L12" s="5"/>
-      <c r="M12" s="5"/>
-      <c r="N12" s="7" t="s">
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="O12" s="6" t="s">
+      <c r="O12" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="P12" s="8">
+      <c r="P12" s="5">
         <v>45173</v>
       </c>
-      <c r="Q12" s="5"/>
+      <c r="Q12" s="2"/>
     </row>
     <row r="13" spans="1:17" ht="56.25" customHeight="1">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="C13" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E13" s="10" t="s">
+      <c r="E13" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="F13" s="6" t="s">
+      <c r="F13" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="5"/>
-      <c r="K13" s="5"/>
-      <c r="L13" s="5"/>
-      <c r="M13" s="5"/>
-      <c r="N13" s="7" t="s">
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="O13" s="6" t="s">
+      <c r="O13" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="P13" s="8">
+      <c r="P13" s="5">
         <v>45173</v>
       </c>
-      <c r="Q13" s="5"/>
+      <c r="Q13" s="2"/>
     </row>
     <row r="14" spans="1:17" ht="110.25" customHeight="1">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="C14" s="12" t="s">
+      <c r="C14" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E14" s="10" t="s">
+      <c r="E14" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="F14" s="6" t="s">
+      <c r="F14" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="5"/>
-      <c r="L14" s="5"/>
-      <c r="M14" s="5"/>
-      <c r="N14" s="7" t="s">
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="O14" s="6" t="s">
+      <c r="O14" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="P14" s="8">
+      <c r="P14" s="5">
         <v>45173</v>
       </c>
-      <c r="Q14" s="5"/>
+      <c r="Q14" s="2"/>
     </row>
     <row r="15" spans="1:17" ht="63.75">
-      <c r="A15" s="9" t="s">
+      <c r="A15" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B15" s="10" t="s">
+      <c r="B15" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="C15" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D15" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E15" s="10" t="s">
+      <c r="E15" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F15" s="6" t="s">
+      <c r="F15" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="5"/>
-      <c r="K15" s="5"/>
-      <c r="L15" s="5"/>
-      <c r="M15" s="5"/>
-      <c r="N15" s="7" t="s">
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="O15" s="6" t="s">
+      <c r="O15" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="P15" s="8">
+      <c r="P15" s="5">
         <v>45173</v>
       </c>
-      <c r="Q15" s="5"/>
-    </row>
-    <row r="16" spans="1:17">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
-      <c r="J16" s="4"/>
-      <c r="K16" s="4"/>
-      <c r="L16" s="4"/>
-      <c r="M16" s="4"/>
-      <c r="N16" s="4"/>
-      <c r="O16" s="4"/>
-      <c r="P16" s="4"/>
-      <c r="Q16" s="4"/>
+      <c r="Q15" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1432,15 +1438,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="df9135bc-a39e-4069-9ffb-360f93402c62" xsi:nil="true"/>
@@ -1449,6 +1446,15 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1667,20 +1673,20 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9A125CC1-1EA7-46BA-BEC6-11D01A40C3E0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6A3C54FB-5819-49BB-95E2-CB49BE3A27CD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="df9135bc-a39e-4069-9ffb-360f93402c62"/>
     <ds:schemaRef ds:uri="48ec3ddf-2ef2-4a9b-9631-68f5ec9f82f4"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9A125CC1-1EA7-46BA-BEC6-11D01A40C3E0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>